<commit_message>
Se agregan resultados de matriz de n = 100 y error de 10^(-8)
</commit_message>
<xml_diff>
--- a/TPE1/Resultados.xlsx
+++ b/TPE1/Resultados.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="116">
   <si>
     <t>1.6071 - 0.0471i</t>
   </si>
@@ -369,6 +369,9 @@
   </si>
   <si>
     <t>n = 100 , Error = 10^(-8)</t>
+  </si>
+  <si>
+    <t>Tiempo: 8.2478e+03 secs</t>
   </si>
 </sst>
 </file>
@@ -412,8 +415,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -709,1467 +715,2070 @@
   <dimension ref="A1:F103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="I101" sqref="I101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="1" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>100</v>
       </c>
+      <c r="E3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>101</v>
       </c>
+      <c r="E4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F4" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>102</v>
       </c>
+      <c r="E5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>103</v>
       </c>
+      <c r="E6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F6" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="E17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="E20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="E21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="E22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="E23" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="E24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="E25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="E26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="E27" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="E28" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="E29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="E30" t="s">
+        <v>27</v>
+      </c>
+      <c r="F30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="E31" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="E32" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="E33" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="E34" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+      <c r="E35" t="s">
+        <v>32</v>
+      </c>
+      <c r="F35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="E36" t="s">
+        <v>33</v>
+      </c>
+      <c r="F36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="E37" t="s">
+        <v>34</v>
+      </c>
+      <c r="F37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+      <c r="E38" t="s">
+        <v>35</v>
+      </c>
+      <c r="F38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+      <c r="E39" t="s">
+        <v>36</v>
+      </c>
+      <c r="F39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
+      <c r="E40" t="s">
+        <v>37</v>
+      </c>
+      <c r="F40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+      <c r="E41" t="s">
+        <v>38</v>
+      </c>
+      <c r="F41" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+      <c r="E42" t="s">
+        <v>39</v>
+      </c>
+      <c r="F42" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+      <c r="E43" t="s">
+        <v>40</v>
+      </c>
+      <c r="F43" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+      <c r="E44" t="s">
+        <v>41</v>
+      </c>
+      <c r="F44" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+      <c r="E45" t="s">
+        <v>42</v>
+      </c>
+      <c r="F45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D46" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+      <c r="E46" t="s">
+        <v>43</v>
+      </c>
+      <c r="F46" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
+      <c r="E47" t="s">
+        <v>44</v>
+      </c>
+      <c r="F47" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
+      <c r="E48" t="s">
+        <v>45</v>
+      </c>
+      <c r="F48" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+      <c r="E49" t="s">
+        <v>46</v>
+      </c>
+      <c r="F49" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D50" s="5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+      <c r="E50" t="s">
+        <v>47</v>
+      </c>
+      <c r="F50" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D51" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
+      <c r="E51" t="s">
+        <v>48</v>
+      </c>
+      <c r="F51" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+      <c r="E52" t="s">
+        <v>49</v>
+      </c>
+      <c r="F52" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D53" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+      <c r="E53" t="s">
+        <v>50</v>
+      </c>
+      <c r="F53" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D54" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+      <c r="E54" t="s">
+        <v>51</v>
+      </c>
+      <c r="F54" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D55" s="5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
+      <c r="E55" t="s">
+        <v>52</v>
+      </c>
+      <c r="F55" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="D56" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
+      <c r="E56" t="s">
+        <v>53</v>
+      </c>
+      <c r="F56" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="D57" s="5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
+      <c r="E57" t="s">
+        <v>54</v>
+      </c>
+      <c r="F57" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="D58" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
+      <c r="E58" t="s">
+        <v>55</v>
+      </c>
+      <c r="F58" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C59" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D59" s="5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
+      <c r="E59" t="s">
+        <v>56</v>
+      </c>
+      <c r="F59" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C60" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D60" s="4" t="s">
+      <c r="D60" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
+      <c r="E60" t="s">
+        <v>57</v>
+      </c>
+      <c r="F60" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C61" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="D61" s="5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
+      <c r="E61" t="s">
+        <v>58</v>
+      </c>
+      <c r="F61" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C62" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="D62" s="5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
+      <c r="E62" t="s">
+        <v>59</v>
+      </c>
+      <c r="F62" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C63" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D63" s="4" t="s">
+      <c r="D63" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
+      <c r="E63" t="s">
+        <v>60</v>
+      </c>
+      <c r="F63" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C64" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="D64" s="5" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
+      <c r="E64" t="s">
+        <v>61</v>
+      </c>
+      <c r="F64" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C65" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="D65" s="5" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
+      <c r="E65" t="s">
+        <v>62</v>
+      </c>
+      <c r="F65" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C66" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D66" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
+      <c r="E66" t="s">
+        <v>63</v>
+      </c>
+      <c r="F66" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C67" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="D67" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
+      <c r="E67" t="s">
+        <v>104</v>
+      </c>
+      <c r="F67" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="C68" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="D68" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
+      <c r="E68" t="s">
+        <v>105</v>
+      </c>
+      <c r="F68" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="C69" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D69" s="4" t="s">
+      <c r="D69" s="5" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
+      <c r="E69" t="s">
+        <v>66</v>
+      </c>
+      <c r="F69" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="C70" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D70" s="4" t="s">
+      <c r="D70" s="5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
+      <c r="E70" t="s">
+        <v>67</v>
+      </c>
+      <c r="F70" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C71" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D71" s="4" t="s">
+      <c r="D71" s="5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
+      <c r="E71" t="s">
+        <v>68</v>
+      </c>
+      <c r="F71" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C72" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D72" s="4" t="s">
+      <c r="D72" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="4" t="s">
+      <c r="E72" t="s">
+        <v>69</v>
+      </c>
+      <c r="F72" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="C73" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D73" s="4" t="s">
+      <c r="D73" s="5" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
+      <c r="E73" t="s">
+        <v>70</v>
+      </c>
+      <c r="F73" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="C74" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D74" s="4" t="s">
+      <c r="D74" s="5" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
+      <c r="E74" t="s">
+        <v>71</v>
+      </c>
+      <c r="F74" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B75" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C75" s="4" t="s">
+      <c r="C75" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D75" s="4" t="s">
+      <c r="D75" s="5" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
+      <c r="E75" t="s">
+        <v>72</v>
+      </c>
+      <c r="F75" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B76" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C76" s="4" t="s">
+      <c r="C76" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D76" s="4" t="s">
+      <c r="D76" s="5" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
+      <c r="E76" t="s">
+        <v>73</v>
+      </c>
+      <c r="F76" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B77" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C77" s="4" t="s">
+      <c r="C77" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D77" s="4" t="s">
+      <c r="D77" s="5" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
+      <c r="E77" t="s">
+        <v>74</v>
+      </c>
+      <c r="F77" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B78" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C78" s="4" t="s">
+      <c r="C78" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D78" s="4" t="s">
+      <c r="D78" s="5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="4" t="s">
+      <c r="E78" t="s">
+        <v>75</v>
+      </c>
+      <c r="F78" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B79" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C79" s="4" t="s">
+      <c r="C79" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D79" s="4" t="s">
+      <c r="D79" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
+      <c r="E79" t="s">
+        <v>76</v>
+      </c>
+      <c r="F79" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C80" s="4" t="s">
+      <c r="C80" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D80" s="4" t="s">
+      <c r="D80" s="5" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="4" t="s">
+      <c r="E80" t="s">
+        <v>77</v>
+      </c>
+      <c r="F80" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B81" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C81" s="4" t="s">
+      <c r="C81" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D81" s="4" t="s">
+      <c r="D81" s="5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
+      <c r="E81" t="s">
+        <v>78</v>
+      </c>
+      <c r="F81" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B82" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C82" s="4" t="s">
+      <c r="C82" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D82" s="4" t="s">
+      <c r="D82" s="5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="4" t="s">
+      <c r="E82" t="s">
+        <v>79</v>
+      </c>
+      <c r="F82" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B83" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C83" s="4" t="s">
+      <c r="C83" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D83" s="4" t="s">
+      <c r="D83" s="5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="4" t="s">
+      <c r="E83" t="s">
+        <v>80</v>
+      </c>
+      <c r="F83" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B84" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C84" s="4" t="s">
+      <c r="C84" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D84" s="4" t="s">
+      <c r="D84" s="5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="4" t="s">
+      <c r="E84" t="s">
+        <v>81</v>
+      </c>
+      <c r="F84" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B85" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C85" s="4" t="s">
+      <c r="C85" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D85" s="4" t="s">
+      <c r="D85" s="5" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="4" t="s">
+      <c r="E85" t="s">
+        <v>82</v>
+      </c>
+      <c r="F85" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B86" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C86" s="4" t="s">
+      <c r="C86" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D86" s="4" t="s">
+      <c r="D86" s="5" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="4" t="s">
+      <c r="E86" t="s">
+        <v>83</v>
+      </c>
+      <c r="F86" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B87" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C87" s="4" t="s">
+      <c r="C87" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D87" s="4" t="s">
+      <c r="D87" s="5" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="4" t="s">
+      <c r="E87" t="s">
+        <v>84</v>
+      </c>
+      <c r="F87" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B88" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C88" s="4" t="s">
+      <c r="C88" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D88" s="4" t="s">
+      <c r="D88" s="5" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="4" t="s">
+      <c r="E88" t="s">
+        <v>85</v>
+      </c>
+      <c r="F88" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B89" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C89" s="4" t="s">
+      <c r="C89" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D89" s="4" t="s">
+      <c r="D89" s="5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="4" t="s">
+      <c r="E89" t="s">
+        <v>86</v>
+      </c>
+      <c r="F89" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B90" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C90" s="4" t="s">
+      <c r="C90" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D90" s="4" t="s">
+      <c r="D90" s="5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="4" t="s">
+      <c r="E90" t="s">
+        <v>87</v>
+      </c>
+      <c r="F90" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B91" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C91" s="4" t="s">
+      <c r="C91" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D91" s="4" t="s">
+      <c r="D91" s="5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="4" t="s">
+      <c r="E91" t="s">
+        <v>88</v>
+      </c>
+      <c r="F91" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B92" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C92" s="4" t="s">
+      <c r="C92" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D92" s="4" t="s">
+      <c r="D92" s="5" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="4" t="s">
+      <c r="E92" t="s">
+        <v>89</v>
+      </c>
+      <c r="F92" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B93" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C93" s="4" t="s">
+      <c r="C93" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D93" s="4" t="s">
+      <c r="D93" s="5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="4" t="s">
+      <c r="E93" t="s">
+        <v>90</v>
+      </c>
+      <c r="F93" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B94" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C94" s="4" t="s">
+      <c r="C94" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D94" s="4" t="s">
+      <c r="D94" s="5" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="4" t="s">
+      <c r="E94" t="s">
+        <v>91</v>
+      </c>
+      <c r="F94" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B95" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C95" s="4" t="s">
+      <c r="C95" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D95" s="4" t="s">
+      <c r="D95" s="5" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="4" t="s">
+      <c r="E95" t="s">
+        <v>92</v>
+      </c>
+      <c r="F95" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B96" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C96" s="4" t="s">
+      <c r="C96" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D96" s="4" t="s">
+      <c r="D96" s="5" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="4" t="s">
+      <c r="E96" t="s">
+        <v>93</v>
+      </c>
+      <c r="F96" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B97" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C97" s="4" t="s">
+      <c r="C97" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D97" s="4" t="s">
+      <c r="D97" s="5" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="4" t="s">
+      <c r="E97" t="s">
+        <v>94</v>
+      </c>
+      <c r="F97" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B98" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C98" s="4" t="s">
+      <c r="C98" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D98" s="4" t="s">
+      <c r="D98" s="5" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="4" t="s">
+      <c r="E98" t="s">
+        <v>95</v>
+      </c>
+      <c r="F98" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B99" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C99" s="4" t="s">
+      <c r="C99" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D99" s="4" t="s">
+      <c r="D99" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="4" t="s">
+      <c r="E99" t="s">
+        <v>96</v>
+      </c>
+      <c r="F99" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B100" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C100" s="4" t="s">
+      <c r="C100" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D100" s="4" t="s">
+      <c r="D100" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="4" t="s">
+      <c r="E100" t="s">
+        <v>97</v>
+      </c>
+      <c r="F100" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B101" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C101" s="4" t="s">
+      <c r="C101" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D101" s="4" t="s">
+      <c r="D101" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="4" t="s">
+      <c r="E101" t="s">
+        <v>98</v>
+      </c>
+      <c r="F101" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B102" s="4" t="s">
+      <c r="B102" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C102" s="4" t="s">
+      <c r="C102" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D102" s="4" t="s">
+      <c r="D102" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
+      <c r="E102" t="s">
+        <v>99</v>
+      </c>
+      <c r="F102" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B103" s="1"/>
-      <c r="C103" s="1" t="s">
+      <c r="B103" s="2"/>
+      <c r="C103" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D103" s="1"/>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F103" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A103:B103"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C103:D103"/>
     <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E103:F103"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
El error queda con 10^(-7) y se emprolijan algunas cosas
</commit_message>
<xml_diff>
--- a/TPE1/Resultados.xlsx
+++ b/TPE1/Resultados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/74a26fb530f5f748/Documents/Facultad/MNA/TPE'S/TPE1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Documents\Facultad\MNA\TPE'S\TPE1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="230">
   <si>
     <t>1.6071 - 0.0471i</t>
   </si>
@@ -372,13 +372,355 @@
   </si>
   <si>
     <t>Tiempo: 8.2478e+03 secs</t>
+  </si>
+  <si>
+    <t>n = 110 , Error = 10^(-7)</t>
+  </si>
+  <si>
+    <t>1.6080 - 0.0433i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6080 + 0.0433i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6086 - 0.1298i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6086 + 0.1298i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6100 - 0.2158i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6100 + 0.2158i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6120 - 0.3011i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6120 + 0.3011i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6147 - 0.3853i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6147 + 0.3853i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6182 - 0.4682i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6182 + 0.4682i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6226 - 0.5493i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6226 + 0.5493i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6278 - 0.6282i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6278 + 0.6282i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.9780 - 1.4710i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.9780 + 1.4710i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.0448 - 1.4255i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.0448 + 1.4255i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.9128 - 1.5176i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.9128 + 1.5176i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.1130 - 1.3816i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.1130 + 1.3816i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6339 - 0.7043i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6339 + 0.7043i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.8497 - 1.5649i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.8497 + 1.5649i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.1824 - 1.3401i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.1824 + 1.3401i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.7885 - 1.6123i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.7885 + 1.6123i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.2522 - 1.3016i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.2522 + 1.3016i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.7296 - 1.6596i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.7296 + 1.6596i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6409 - 0.7772i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6409 + 0.7772i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.3218 - 1.2668i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.3218 + 1.2668i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.6729 - 1.7065i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.6729 + 1.7065i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6488 - 0.8461i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6488 + 0.8461i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.6185 - 1.7525i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.6185 + 1.7525i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.3900 - 1.2365i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.3900 + 1.2365i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.5664 - 1.7975i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.5664 + 1.7975i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6573 - 0.9102i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6573 + 0.9102i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.4556 - 1.2111i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.4556 + 1.2111i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.5168 - 1.8412i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.5168 + 1.8412i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6661 - 0.9686i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6661 + 0.9686i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.5166 - 1.1909i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.5166 + 1.1909i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.4696 - 1.8835i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.4696 + 1.8835i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6745 - 1.0203i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6745 + 1.0203i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.5709 - 1.1755i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.5709 + 1.1755i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.4249 - 1.9242i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.4249 + 1.9242i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6815 - 1.0642i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6815 + 1.0642i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6163 - 1.1638i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6163 + 1.1638i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.3827 - 1.9630i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.3827 + 1.9630i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6853 - 1.0993i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6853 + 1.0993i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6508 - 1.1538i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6508 + 1.1538i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6836 - 1.1251i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6836 + 1.1251i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6731 - 1.1422i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6731 + 1.1422i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.3431 - 2.0000i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.3431 + 2.0000i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.3061 - 2.0349i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.3061 + 2.0349i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.2716 - 2.0676i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.2716 + 2.0676i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.2398 - 2.0980i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.2398 + 2.0980i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.2107 - 2.1261i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.2107 + 2.1261i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.1843 - 2.1517i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.1843 + 2.1517i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.1606 - 2.1749i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.1606 + 2.1749i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.1396 - 2.1954i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.1396 + 2.1954i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.1214 - 2.2133i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.1214 + 2.2133i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.1059 - 2.2286i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.1059 + 2.2286i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.0933 - 2.2411i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.0933 + 2.2411i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.0834 - 2.2509i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.0834 + 2.2509i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.0764 - 2.2579i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.0764 + 2.2579i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.0721 - 2.2621i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.0721 + 2.2621i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.9779 - 1.4710i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.9779 + 1.4710i</t>
+  </si>
+  <si>
+    <t>Tiempo: 579.0750 secs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -394,19 +736,71 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -415,14 +809,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -430,8 +818,28 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,2067 +1120,2765 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F103"/>
+  <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I101" sqref="I101"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="I95" sqref="I95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="5"/>
+      <c r="E1" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="6" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="G2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="9" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="G3" t="s">
+        <v>117</v>
+      </c>
+      <c r="H3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="11" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="G4" t="s">
+        <v>118</v>
+      </c>
+      <c r="H4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="11" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="G5" t="s">
+        <v>119</v>
+      </c>
+      <c r="H5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="11" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="G6" t="s">
+        <v>120</v>
+      </c>
+      <c r="H6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="G7" t="s">
+        <v>121</v>
+      </c>
+      <c r="H7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="G8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="G9" t="s">
+        <v>123</v>
+      </c>
+      <c r="H9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="G10" t="s">
+        <v>124</v>
+      </c>
+      <c r="H10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="G11" t="s">
+        <v>125</v>
+      </c>
+      <c r="H11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="G12" t="s">
+        <v>126</v>
+      </c>
+      <c r="H12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="G13" t="s">
+        <v>127</v>
+      </c>
+      <c r="H13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="G14" t="s">
+        <v>128</v>
+      </c>
+      <c r="H14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="G15" t="s">
+        <v>129</v>
+      </c>
+      <c r="H15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="G16" t="s">
+        <v>130</v>
+      </c>
+      <c r="H16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="G17" t="s">
+        <v>131</v>
+      </c>
+      <c r="H17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="G18" t="s">
+        <v>132</v>
+      </c>
+      <c r="H18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="G19" t="s">
+        <v>133</v>
+      </c>
+      <c r="H19" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="G20" t="s">
+        <v>134</v>
+      </c>
+      <c r="H20" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="G21" t="s">
+        <v>135</v>
+      </c>
+      <c r="H21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="G22" t="s">
+        <v>136</v>
+      </c>
+      <c r="H22" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="G23" t="s">
+        <v>137</v>
+      </c>
+      <c r="H23" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="G24" t="s">
+        <v>138</v>
+      </c>
+      <c r="H24" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+      <c r="G25" t="s">
+        <v>139</v>
+      </c>
+      <c r="H25" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="11" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="G26" t="s">
+        <v>140</v>
+      </c>
+      <c r="H26" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="11" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="G27" t="s">
+        <v>141</v>
+      </c>
+      <c r="H27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="11" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="G28" t="s">
+        <v>142</v>
+      </c>
+      <c r="H28" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="11" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="G29" t="s">
+        <v>143</v>
+      </c>
+      <c r="H29" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="G30" t="s">
+        <v>144</v>
+      </c>
+      <c r="H30" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+      <c r="G31" t="s">
+        <v>145</v>
+      </c>
+      <c r="H31" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="11" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+      <c r="G32" t="s">
+        <v>146</v>
+      </c>
+      <c r="H32" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+      <c r="G33" t="s">
+        <v>147</v>
+      </c>
+      <c r="H33" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="11" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+      <c r="G34" t="s">
+        <v>148</v>
+      </c>
+      <c r="H34" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+      <c r="G35" t="s">
+        <v>149</v>
+      </c>
+      <c r="H35" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+      <c r="G36" t="s">
+        <v>150</v>
+      </c>
+      <c r="H36" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="11" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+      <c r="G37" t="s">
+        <v>151</v>
+      </c>
+      <c r="H37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="11" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+      <c r="G38" t="s">
+        <v>152</v>
+      </c>
+      <c r="H38" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="11" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+      <c r="G39" t="s">
+        <v>153</v>
+      </c>
+      <c r="H39" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="11" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+      <c r="G40" t="s">
+        <v>154</v>
+      </c>
+      <c r="H40" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="11" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
+      <c r="G41" t="s">
+        <v>155</v>
+      </c>
+      <c r="H41" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="11" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+      <c r="G42" t="s">
+        <v>156</v>
+      </c>
+      <c r="H42" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="11" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+      <c r="G43" t="s">
+        <v>157</v>
+      </c>
+      <c r="H43" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="11" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
+      <c r="G44" t="s">
+        <v>158</v>
+      </c>
+      <c r="H44" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45" s="11" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
+      <c r="G45" t="s">
+        <v>159</v>
+      </c>
+      <c r="H45" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
+      <c r="G46" t="s">
+        <v>160</v>
+      </c>
+      <c r="H46" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="11" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
+      <c r="G47" t="s">
+        <v>161</v>
+      </c>
+      <c r="H47" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D48" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F48" s="11" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
+      <c r="G48" t="s">
+        <v>162</v>
+      </c>
+      <c r="H48" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C49" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" s="11" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
+      <c r="G49" t="s">
+        <v>163</v>
+      </c>
+      <c r="H49" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C50" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D50" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50" s="11" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
+      <c r="G50" t="s">
+        <v>164</v>
+      </c>
+      <c r="H50" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C51" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D51" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51" s="11" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
+      <c r="G51" t="s">
+        <v>165</v>
+      </c>
+      <c r="H51" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C52" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="D52" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F52" s="11" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
+      <c r="G52" t="s">
+        <v>166</v>
+      </c>
+      <c r="H52" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C53" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="D53" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" s="11" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
+      <c r="G53" t="s">
+        <v>167</v>
+      </c>
+      <c r="H53" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C54" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D54" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" s="11" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
+      <c r="G54" t="s">
+        <v>168</v>
+      </c>
+      <c r="H54" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C55" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D55" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
+      <c r="G55" t="s">
+        <v>169</v>
+      </c>
+      <c r="H55" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C56" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="D56" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" s="11" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
+      <c r="G56" t="s">
+        <v>170</v>
+      </c>
+      <c r="H56" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B57" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C57" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="D57" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57" s="11" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
+      <c r="G57" t="s">
+        <v>171</v>
+      </c>
+      <c r="H57" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="C58" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="D58" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F58" s="11" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
+      <c r="G58" t="s">
+        <v>172</v>
+      </c>
+      <c r="H58" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B59" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C59" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="D59" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E59" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F59" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
+      <c r="G59" t="s">
+        <v>173</v>
+      </c>
+      <c r="H59" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C60" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D60" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F60" s="11" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
+      <c r="G60" t="s">
+        <v>174</v>
+      </c>
+      <c r="H60" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C61" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="D61" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F61" s="11" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
+      <c r="G61" t="s">
+        <v>175</v>
+      </c>
+      <c r="H61" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C62" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E62" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F62" s="11" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
+      <c r="G62" t="s">
+        <v>176</v>
+      </c>
+      <c r="H62" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="C63" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D63" s="5" t="s">
+      <c r="D63" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F63" s="11" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
+      <c r="G63" t="s">
+        <v>177</v>
+      </c>
+      <c r="H63" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C64" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="D64" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F64" s="11" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="5" t="s">
+      <c r="G64" t="s">
+        <v>178</v>
+      </c>
+      <c r="H64" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C65" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="D65" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E65" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F65" s="11" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
+      <c r="G65" t="s">
+        <v>179</v>
+      </c>
+      <c r="H65" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C66" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="D66" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E66" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F66" s="11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="5" t="s">
+      <c r="G66" t="s">
+        <v>180</v>
+      </c>
+      <c r="H66" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="C67" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="D67" s="5" t="s">
+      <c r="D67" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E67" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F67" s="11" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="5" t="s">
+      <c r="G67" t="s">
+        <v>181</v>
+      </c>
+      <c r="H67" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C68" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D68" s="5" t="s">
+      <c r="D68" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E68" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F68" s="11" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="5" t="s">
+      <c r="G68" t="s">
+        <v>182</v>
+      </c>
+      <c r="H68" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C69" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="D69" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E69" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F69" s="11" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
+      <c r="G69" t="s">
+        <v>183</v>
+      </c>
+      <c r="H69" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C70" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="D70" s="5" t="s">
+      <c r="D70" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E70" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F70" s="11" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
+      <c r="G70" t="s">
+        <v>184</v>
+      </c>
+      <c r="H70" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B71" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C71" s="5" t="s">
+      <c r="C71" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D71" s="5" t="s">
+      <c r="D71" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E71" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F71" s="11" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
+      <c r="G71" t="s">
+        <v>185</v>
+      </c>
+      <c r="H71" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C72" s="5" t="s">
+      <c r="C72" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D72" s="5" t="s">
+      <c r="D72" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E72" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F72" t="s">
+      <c r="F72" s="11" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
+      <c r="G72" t="s">
+        <v>186</v>
+      </c>
+      <c r="H72" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B73" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="C73" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D73" s="5" t="s">
+      <c r="D73" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E73" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F73" s="11" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
+      <c r="G73" t="s">
+        <v>187</v>
+      </c>
+      <c r="H73" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C74" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="D74" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E74" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="F74" t="s">
+      <c r="F74" s="11" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
+      <c r="G74" t="s">
+        <v>188</v>
+      </c>
+      <c r="H74" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C75" s="5" t="s">
+      <c r="C75" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="D75" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E75" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F75" s="11" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
+      <c r="G75" t="s">
+        <v>189</v>
+      </c>
+      <c r="H75" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B76" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="C76" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="D76" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E76" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F76" s="11" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="5" t="s">
+      <c r="G76" t="s">
+        <v>190</v>
+      </c>
+      <c r="H76" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C77" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D77" s="5" t="s">
+      <c r="D77" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F77" s="11" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="5" t="s">
+      <c r="G77" t="s">
+        <v>191</v>
+      </c>
+      <c r="H77" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B78" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C78" s="5" t="s">
+      <c r="C78" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D78" s="5" t="s">
+      <c r="D78" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E78" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F78" s="11" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="5" t="s">
+      <c r="G78" t="s">
+        <v>192</v>
+      </c>
+      <c r="H78" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B79" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C79" s="5" t="s">
+      <c r="C79" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="D79" s="5" t="s">
+      <c r="D79" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E79" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F79" s="11" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="5" t="s">
+      <c r="G79" t="s">
+        <v>193</v>
+      </c>
+      <c r="H79" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B80" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C80" s="5" t="s">
+      <c r="C80" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D80" s="5" t="s">
+      <c r="D80" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E80" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F80" s="11" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
+      <c r="G80" t="s">
+        <v>194</v>
+      </c>
+      <c r="H80" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B81" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C81" s="5" t="s">
+      <c r="C81" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D81" s="5" t="s">
+      <c r="D81" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E81" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F81" s="11" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="5" t="s">
+      <c r="G81" t="s">
+        <v>195</v>
+      </c>
+      <c r="H81" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="B82" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C82" s="5" t="s">
+      <c r="C82" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D82" s="5" t="s">
+      <c r="D82" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E82" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F82" s="11" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="5" t="s">
+      <c r="G82" t="s">
+        <v>196</v>
+      </c>
+      <c r="H82" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B83" s="5" t="s">
+      <c r="B83" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C83" s="5" t="s">
+      <c r="C83" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D83" s="5" t="s">
+      <c r="D83" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E83" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F83" s="11" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="5" t="s">
+      <c r="G83" t="s">
+        <v>197</v>
+      </c>
+      <c r="H83" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="B84" s="5" t="s">
+      <c r="B84" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C84" s="5" t="s">
+      <c r="C84" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D84" s="5" t="s">
+      <c r="D84" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E84" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F84" s="11" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="5" t="s">
+      <c r="G84" t="s">
+        <v>198</v>
+      </c>
+      <c r="H84" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B85" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C85" s="5" t="s">
+      <c r="C85" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="D85" s="5" t="s">
+      <c r="D85" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E85" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="F85" t="s">
+      <c r="F85" s="11" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="5" t="s">
+      <c r="G85" t="s">
+        <v>199</v>
+      </c>
+      <c r="H85" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B86" s="5" t="s">
+      <c r="B86" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C86" s="5" t="s">
+      <c r="C86" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D86" s="5" t="s">
+      <c r="D86" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="E86" t="s">
+      <c r="E86" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F86" s="11" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="5" t="s">
+      <c r="G86" t="s">
+        <v>200</v>
+      </c>
+      <c r="H86" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B87" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C87" s="5" t="s">
+      <c r="C87" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D87" s="5" t="s">
+      <c r="D87" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="E87" t="s">
+      <c r="E87" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="F87" t="s">
+      <c r="F87" s="11" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="5" t="s">
+      <c r="G87" t="s">
+        <v>201</v>
+      </c>
+      <c r="H87" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B88" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C88" s="5" t="s">
+      <c r="C88" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="D88" s="5" t="s">
+      <c r="D88" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="E88" t="s">
+      <c r="E88" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="F88" t="s">
+      <c r="F88" s="11" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="5" t="s">
+      <c r="G88" t="s">
+        <v>202</v>
+      </c>
+      <c r="H88" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="B89" s="5" t="s">
+      <c r="B89" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C89" s="5" t="s">
+      <c r="C89" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="D89" s="5" t="s">
+      <c r="D89" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="E89" t="s">
+      <c r="E89" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="F89" t="s">
+      <c r="F89" s="11" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="5" t="s">
+      <c r="G89" t="s">
+        <v>203</v>
+      </c>
+      <c r="H89" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="B90" s="5" t="s">
+      <c r="B90" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C90" s="5" t="s">
+      <c r="C90" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D90" s="5" t="s">
+      <c r="D90" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E90" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="F90" t="s">
+      <c r="F90" s="11" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="5" t="s">
+      <c r="G90" t="s">
+        <v>204</v>
+      </c>
+      <c r="H90" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B91" s="5" t="s">
+      <c r="B91" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="C91" s="5" t="s">
+      <c r="C91" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D91" s="5" t="s">
+      <c r="D91" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="E91" t="s">
+      <c r="E91" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="F91" t="s">
+      <c r="F91" s="11" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="5" t="s">
+      <c r="G91" t="s">
+        <v>205</v>
+      </c>
+      <c r="H91" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="B92" s="5" t="s">
+      <c r="B92" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C92" s="5" t="s">
+      <c r="C92" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D92" s="5" t="s">
+      <c r="D92" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E92" t="s">
+      <c r="E92" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="F92" t="s">
+      <c r="F92" s="11" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="5" t="s">
+      <c r="G92" t="s">
+        <v>206</v>
+      </c>
+      <c r="H92" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B93" s="5" t="s">
+      <c r="B93" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C93" s="5" t="s">
+      <c r="C93" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D93" s="5" t="s">
+      <c r="D93" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="E93" t="s">
+      <c r="E93" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="F93" t="s">
+      <c r="F93" s="11" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="5" t="s">
+      <c r="G93" t="s">
+        <v>207</v>
+      </c>
+      <c r="H93" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B94" s="5" t="s">
+      <c r="B94" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="C94" s="5" t="s">
+      <c r="C94" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D94" s="5" t="s">
+      <c r="D94" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="E94" t="s">
+      <c r="E94" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="F94" t="s">
+      <c r="F94" s="11" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="5" t="s">
+      <c r="G94" t="s">
+        <v>208</v>
+      </c>
+      <c r="H94" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B95" s="5" t="s">
+      <c r="B95" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="C95" s="5" t="s">
+      <c r="C95" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D95" s="5" t="s">
+      <c r="D95" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="E95" t="s">
+      <c r="E95" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="F95" t="s">
+      <c r="F95" s="11" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="5" t="s">
+      <c r="G95" t="s">
+        <v>209</v>
+      </c>
+      <c r="H95" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="B96" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C96" s="5" t="s">
+      <c r="C96" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D96" s="5" t="s">
+      <c r="D96" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E96" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="F96" t="s">
+      <c r="F96" s="11" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="5" t="s">
+      <c r="G96" t="s">
+        <v>210</v>
+      </c>
+      <c r="H96" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B97" s="5" t="s">
+      <c r="B97" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C97" s="5" t="s">
+      <c r="C97" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D97" s="5" t="s">
+      <c r="D97" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E97" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="F97" t="s">
+      <c r="F97" s="11" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="5" t="s">
+      <c r="G97" t="s">
+        <v>211</v>
+      </c>
+      <c r="H97" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="B98" s="5" t="s">
+      <c r="B98" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C98" s="5" t="s">
+      <c r="C98" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="D98" s="5" t="s">
+      <c r="D98" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="E98" t="s">
+      <c r="E98" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="F98" t="s">
+      <c r="F98" s="11" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="5" t="s">
+      <c r="G98" t="s">
+        <v>212</v>
+      </c>
+      <c r="H98" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B99" s="5" t="s">
+      <c r="B99" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="C99" s="5" t="s">
+      <c r="C99" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="D99" s="5" t="s">
+      <c r="D99" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E99" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="F99" t="s">
+      <c r="F99" s="11" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="5" t="s">
+      <c r="G99" t="s">
+        <v>213</v>
+      </c>
+      <c r="H99" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="B100" s="5" t="s">
+      <c r="B100" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="C100" s="5" t="s">
+      <c r="C100" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="D100" s="5" t="s">
+      <c r="D100" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="E100" t="s">
+      <c r="E100" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="F100" t="s">
+      <c r="F100" s="11" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="5" t="s">
+      <c r="G100" t="s">
+        <v>214</v>
+      </c>
+      <c r="H100" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="B101" s="5" t="s">
+      <c r="B101" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C101" s="5" t="s">
+      <c r="C101" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="D101" s="5" t="s">
+      <c r="D101" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E101" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="F101" t="s">
+      <c r="F101" s="11" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="5" t="s">
+      <c r="G101" t="s">
+        <v>215</v>
+      </c>
+      <c r="H101" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B102" s="5" t="s">
+      <c r="B102" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="C102" s="5" t="s">
+      <c r="C102" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="D102" s="5" t="s">
+      <c r="D102" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="E102" t="s">
+      <c r="E102" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="F102" t="s">
+      <c r="F102" s="11" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
+      <c r="G102" t="s">
+        <v>216</v>
+      </c>
+      <c r="H102" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B103" s="2"/>
-      <c r="C103" s="2" t="s">
+      <c r="B103" s="4"/>
+      <c r="C103" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D103" s="2"/>
-      <c r="E103" s="2" t="s">
+      <c r="D103" s="4"/>
+      <c r="E103" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F103" s="1"/>
+      <c r="F103" s="7"/>
+      <c r="G103" t="s">
+        <v>217</v>
+      </c>
+      <c r="H103" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G104" t="s">
+        <v>218</v>
+      </c>
+      <c r="H104" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G105" t="s">
+        <v>219</v>
+      </c>
+      <c r="H105" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G106" t="s">
+        <v>220</v>
+      </c>
+      <c r="H106" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G107" t="s">
+        <v>221</v>
+      </c>
+      <c r="H107" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G108" t="s">
+        <v>222</v>
+      </c>
+      <c r="H108" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G109" t="s">
+        <v>223</v>
+      </c>
+      <c r="H109" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G110" t="s">
+        <v>224</v>
+      </c>
+      <c r="H110" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G111" t="s">
+        <v>225</v>
+      </c>
+      <c r="H111" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G112" t="s">
+        <v>226</v>
+      </c>
+      <c r="H112" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="113" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G113" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="H113" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G113:H113"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A103:B103"/>
     <mergeCell ref="C1:D1"/>

</xml_diff>